<commit_message>
Added condition that make sure that both test have tthe same similiarity score before appending to a new dataframe
</commit_message>
<xml_diff>
--- a/matchv1.xlsx
+++ b/matchv1.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I9"/>
+  <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -477,241 +477,249 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>2023052003089</v>
+        <v>2023052003075</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>RSV PCR</t>
+          <t>SARSCoV2 PCR</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Respiratory syncytial virus RNA Presence Respiratory Specimen NAA Probe Detection</t>
+          <t>SARS Coronavirus+SARS-like Coronavirus+SARS Coronavirus 2 RNA Presence Resp Spec NAA Probe Detection</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>['rsv', 'pcr']</t>
+          <t>['sarscov2', 'pcr']</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>['respiratory', 'syncytial', 'virus', 'rna', 'presence', 'respiratory', 'specimen', 'naa', 'probe', 'detection']</t>
+          <t>['sars', 'coronavirus+sars-like', 'coronavirus+sars', 'coronavirus', '2', 'rna', 'presence', 'resp', 'spec', 'naa', 'probe', 'detection']</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>[ 0.02942644  0.02310146  0.03788712  0.05792619 -0.00295022 -0.02871712
-  0.05042725  0.06419385 -0.07061685 -0.0698652  -0.01642724 -0.04401613
-  0.02589053  0.01977798  0.02794593 -0.00664669  0.08338402 -0.01608654
- -0.03128926 -0.1356791   0.03495158  0.02010236  0.04145234 -0.05478261
- -0.07260284  0.04122154 -0.08095238  0.04129557 -0.00637056  0.04196689
-  0.03239698 -0.03096748 -0.0204769  -0.07187746 -0.03373796  0.02766523
-  0.0222581   0.0142471  -0.06437353 -0.01040409  0.05364886 -0.03603682
- -0.00311126  0.05118546  0.025288   -0.05460387 -0.05635084 -0.04811082
-  0.0597598   0.02091271 -0.01993456 -0.06124961  0.01316796 -0.01368303
- -0.04713557  0.05873607  0.01293273  0.00520588  0.01099207  0.01626415
-  0.01213544 -0.04588237  0.06883674  0.05246281 -0.02916823  0.10275106
- -0.01603425  0.06594267 -0.06442071 -0.00644601  0.00458856  0.04429123
-  0.03980447  0.00202958  0.02836489  0.00853634  0.04424687  0.04772226
- -0.02150173 -0.04826249 -0.0926463   0.00270346 -0.02400313  0.04637054
-  0.00651246 -0.02949534  0.03395392  0.036445    0.03593185 -0.00092523
-  0.0540988  -0.00343172 -0.02609881  0.01937107  0.04933371 -0.0071256
-  0.01996965 -0.019446    0.01732027  0.03822035]</t>
+          <t>[ 0.04844983  0.04097991  0.05468198  0.08553599 -0.00717009 -0.04813475
+  0.06729161  0.10693806 -0.11113567 -0.10656811 -0.02301322 -0.05408894
+  0.0372901   0.02567828  0.05225355 -0.01311089  0.1136051  -0.02536148
+ -0.04379593 -0.20972255  0.05115614  0.0115237   0.05966483 -0.08953157
+ -0.11238225  0.05254484 -0.1188067   0.06567574  0.00179666  0.06146365
+  0.04121104 -0.04933323 -0.02536683 -0.09700932 -0.04425994  0.04964492
+  0.03558797  0.01398294 -0.10518108 -0.01832112  0.07263307 -0.05073287
+  0.00448335  0.08507431  0.0344374  -0.08297727 -0.06398692 -0.07187506
+  0.07906107  0.03469941 -0.02080077 -0.08831837  0.01699595 -0.00834517
+ -0.077101    0.08191757  0.01804875  0.01130721  0.01631725  0.01247251
+  0.01946101 -0.06136871  0.10084354  0.07152377 -0.04764863  0.1579251
+ -0.00419722  0.09928529 -0.10342035 -0.00135123 -0.00107175  0.07134499
+  0.0546937   0.01383806  0.04896311  0.02521991  0.06213642  0.08400159
+ -0.03577693 -0.06506013 -0.13255027  0.01738206 -0.04213398  0.06469294
+  0.01047818 -0.03613191  0.04438787  0.04281722  0.05252972  0.00609954
+  0.08188532 -0.00877357 -0.04751994  0.03520501  0.07726957 -0.0210616
+  0.01935977 -0.03133991  0.02572532  0.05920391]</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>[ 4.90662046e-02  1.22415945e-01  1.23210728e-01  1.84805542e-01
-  4.59339283e-03 -1.23377047e-01  1.83278084e-01  3.02326858e-01
- -2.73575127e-01 -2.61368126e-01 -6.11181855e-02 -1.80040702e-01
-  8.05611014e-02  8.00925121e-02  1.23520926e-01 -2.47075912e-02
-  3.03895533e-01 -3.85379754e-02 -9.29595530e-02 -5.26447356e-01
-  1.64968342e-01  4.54637632e-02  1.85307011e-01 -1.83010504e-01
- -2.43202418e-01  1.54329345e-01 -2.78595626e-01  1.30578890e-01
-  7.84613751e-03  1.25963047e-01  1.44847348e-01 -1.33442342e-01
- -5.38146570e-02 -2.46053860e-01 -1.07868649e-01  1.44562781e-01
-  1.30162358e-01  4.80633974e-02 -2.37953022e-01 -3.45979892e-02
-  2.03784585e-01 -1.32429048e-01 -3.73820774e-03  2.02232286e-01
-  8.43675509e-02 -1.82519525e-01 -1.89610034e-01 -1.86494187e-01
-  1.86460942e-01  6.32078722e-02 -3.15692164e-02 -2.15600580e-01
- -3.29441996e-03 -2.17773281e-02 -1.71120435e-01  1.73244059e-01
-  9.13885906e-02 -8.01325589e-03  4.79256511e-02  3.02239116e-02
-  8.38989671e-03 -1.64157107e-01  2.94999272e-01  1.66612715e-01
- -1.15381852e-01  3.81726682e-01 -5.50877023e-03  2.32572287e-01
- -2.46131927e-01  7.54625816e-03 -3.58191878e-03  1.65737182e-01
-  1.38137743e-01  5.12560233e-02  1.43335968e-01  3.82832363e-02
-  1.66509390e-01  2.09597751e-01 -9.87995490e-02 -1.40422180e-01
- -3.39652956e-01  8.15592706e-03 -4.97914404e-02  1.68829113e-01
- -9.58916731e-03 -9.06352773e-02  1.40676469e-01  8.81583616e-02
-  8.40572193e-02 -1.67195540e-04  2.02545643e-01  1.59681831e-02
- -5.21735251e-02  4.89713326e-02  2.15942189e-01 -1.46093685e-02
-  9.69690830e-02 -6.23106882e-02  7.39831626e-02  1.82518691e-01]</t>
+          <t>[ 2.99221147e-02  1.03954159e-01  1.15190476e-01  1.70237735e-01
+ -9.24916286e-03 -1.16083525e-01  1.71648994e-01  2.88631946e-01
+ -2.73772031e-01 -2.61409819e-01 -5.14109731e-02 -1.57738686e-01
+  8.54621902e-02  6.48749918e-02  1.36029750e-01 -2.11676061e-02
+  3.07783931e-01 -4.42240126e-02 -8.93947780e-02 -5.12431681e-01
+  1.43472880e-01  3.92976962e-02  2.07755864e-01 -1.66864038e-01
+ -2.07617655e-01  1.54489219e-01 -2.89462149e-01  1.33851171e-01
+  9.15572327e-03  1.38254583e-01  1.57219321e-01 -1.10909589e-01
+ -3.12280357e-02 -2.14093551e-01 -9.95291397e-02  1.29718438e-01
+  1.03058912e-01  4.53612059e-02 -2.10352883e-01 -4.70763855e-02
+  1.73520684e-01 -1.00697435e-01 -7.36497948e-03  1.75518319e-01
+  5.09812199e-02 -2.00088933e-01 -1.67289600e-01 -1.55999362e-01
+  1.60037607e-01  6.48457259e-02 -2.90617365e-02 -2.07897946e-01
+ -3.88999172e-02 -2.27546189e-02 -1.55136541e-01  1.46816432e-01
+  6.72741607e-02 -1.00608030e-02  6.64832070e-02  2.17609834e-02
+ -9.21988208e-03 -1.51559293e-01  3.19240898e-01  1.57861724e-01
+ -1.44274905e-01  3.62334639e-01  5.82315214e-03  2.03267828e-01
+ -2.63387233e-01 -1.72018845e-04  8.71438440e-03  1.84498206e-01
+  1.15185581e-01  5.37278205e-02  1.30814001e-01  3.53452452e-02
+  1.47847787e-01  1.84367403e-01 -1.18797421e-01 -1.30004659e-01
+ -3.06758851e-01  8.21810123e-03 -2.57283654e-02  2.02897429e-01
+ -1.42591884e-02 -9.96511355e-02  1.40742317e-01  9.23444554e-02
+  6.88763484e-02  4.98412410e-03  1.85781002e-01  1.68066081e-02
+ -4.31126989e-02  4.72450405e-02  2.23643109e-01 -2.07959898e-02
+  1.16742261e-01 -6.73903450e-02  9.41318795e-02  1.67366609e-01]</t>
         </is>
       </c>
       <c r="I2" t="n">
-        <v>0.9865148067474365</v>
+        <v>0.9795011281967163</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B3" t="n">
-        <v>2023046001084</v>
+        <v>2023052003089</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>SARS-CoV-2 (In-house)</t>
+          <t>RSV PCR</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>SARS Coronavirus 2 N gene Presence Respiratory Specimen NAA Probe Detection</t>
+          <t>SARS Coronavirus+SARS-like Coronavirus+SARS Coronavirus 2 RNA Presence Resp Spec NAA Probe Detection</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>['sars-cov-2', '(in-house)']</t>
+          <t>['rsv', 'pcr']</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>['sars', 'coronavirus', '2', 'n', 'gene', 'presence', 'respiratory', 'specimen', 'naa', 'probe', 'detection']</t>
+          <t>['sars', 'coronavirus+sars-like', 'coronavirus+sars', 'coronavirus', '2', 'rna', 'presence', 'resp', 'spec', 'naa', 'probe', 'detection']</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>[ 0.04099466  0.0303609   0.03720009  0.07238427 -0.00606999 -0.03834579
-  0.0698202   0.10011606 -0.09731568 -0.09968016 -0.02777917 -0.05304668
-  0.04094192  0.03688332  0.05247553 -0.00546684  0.11286746 -0.01439495
- -0.02683878 -0.17354727  0.05533121  0.01068354  0.04247902 -0.0737656
- -0.08675258  0.05496167 -0.11086813  0.04513546  0.0184927   0.05317676
-  0.05151162 -0.04630691 -0.02044388 -0.0810457  -0.04515058  0.05059026
-  0.03172128  0.014218   -0.07712391 -0.02825587  0.06444962 -0.0381052
-  0.01664546  0.08230937  0.01944799 -0.06558254 -0.06923109 -0.07098615
-  0.0772863   0.02141471 -0.02823018 -0.08549069 -0.01352204 -0.01145078
- -0.04971896  0.0833569   0.02468219  0.00675989  0.0365702   0.00981783
-  0.00618279 -0.05267407  0.10457907  0.06595862 -0.04543764  0.14707077
- -0.00337199  0.07919507 -0.09340242  0.00158731  0.00232079  0.05433181
-  0.0521543   0.0100879   0.05111912  0.01229095  0.05637821  0.08297427
- -0.04576781 -0.0585273  -0.12425321  0.00659157 -0.02248288  0.06868863
-  0.01752669 -0.03223498  0.04429401  0.03250419  0.02792315 -0.01478605
-  0.07537998 -0.00343691 -0.02983456  0.04082518  0.05882058 -0.01892177
-  0.02416473 -0.01684804  0.03390396  0.07001458]</t>
+          <t>[ 0.02942837  0.02310598  0.03789014  0.05793071 -0.00295052 -0.0287213
+  0.05043221  0.0642042  -0.07062522 -0.06987356 -0.01643042 -0.04402154
+  0.02589212  0.01977976  0.02794919 -0.00664891  0.08339321 -0.01608785
+ -0.03129214 -0.1356954   0.03495633  0.02010256  0.0414561  -0.05478788
+ -0.07261184  0.04122494 -0.08095991  0.04130065 -0.00637076  0.04197177
+  0.03240032 -0.03097287 -0.02048014 -0.07188752 -0.03374127  0.02766968
+  0.0222634   0.01424906 -0.06438092 -0.0104038   0.05365547 -0.0360419
+ -0.00311208  0.05119356  0.02529144 -0.05460997 -0.05635663 -0.04811657
+  0.05976688  0.02091521 -0.01993524 -0.06125603  0.01316957 -0.01368368
+ -0.0471418   0.05874256  0.01293677  0.00520562  0.01099234  0.01626586
+  0.01213747 -0.04588756  0.06884496  0.05246773 -0.02917127  0.10276646
+ -0.01603282  0.06595273 -0.06442957 -0.00644588  0.00458949  0.04429734
+  0.03981029  0.00203076  0.02837091  0.00854021  0.04425386  0.04773219
+ -0.02150447 -0.04826829 -0.09266023  0.00270468 -0.02400529  0.04637613
+  0.00651211 -0.02949909  0.03395872  0.03644961  0.0359362  -0.00092551
+  0.05410795 -0.00343079 -0.02610091  0.01937274  0.04934253 -0.00712683
+  0.01997229 -0.01944889  0.01732302  0.03822708]</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>[ 0.04662418  0.11957259  0.12045899  0.17555206  0.00536327 -0.12201626
-  0.1779787   0.29735506 -0.26796263 -0.25333416 -0.06293678 -0.17655645
-  0.07179141  0.07998554  0.11570292 -0.02764251  0.29166764 -0.03511026
- -0.08861118 -0.5141267   0.16170782  0.04063639  0.18057813 -0.17605722
- -0.2416032   0.15091562 -0.26572374  0.12336297  0.00473609  0.12277524
-  0.14029938 -0.13092686 -0.05781277 -0.24643937 -0.10126564  0.14556961
-  0.12778006  0.04412977 -0.23535174 -0.03328854  0.20545502 -0.13942899
- -0.00627199  0.20077023  0.08853637 -0.17313442 -0.1870845  -0.18521981
-  0.18430196  0.05793643 -0.02978812 -0.21100907  0.00367519 -0.01756596
- -0.16947572  0.16949266  0.09040598 -0.01362792  0.04040028  0.02835724
-  0.01384658 -0.16048227  0.2811318   0.16119474 -0.10282965  0.3716408
- -0.00522976  0.23281954 -0.23541537  0.00619706 -0.0032783   0.16250068
-  0.13563313  0.0523052   0.14347902  0.04078978  0.1640548   0.20902768
- -0.08624148 -0.13662075 -0.3306854   0.00614111 -0.05053623  0.15552904
- -0.01127073 -0.09036312  0.13656001  0.08548255  0.08312407 -0.00247394
-  0.20230912  0.01722513 -0.0507563   0.04478792  0.20748848 -0.01029764
-  0.09211721 -0.06328379  0.06751848  0.17719975]</t>
+          <t>[ 2.99221147e-02  1.03954159e-01  1.15190476e-01  1.70237735e-01
+ -9.24916286e-03 -1.16083525e-01  1.71648994e-01  2.88631946e-01
+ -2.73772031e-01 -2.61409819e-01 -5.14109731e-02 -1.57738686e-01
+  8.54621902e-02  6.48749918e-02  1.36029750e-01 -2.11676061e-02
+  3.07783931e-01 -4.42240126e-02 -8.93947780e-02 -5.12431681e-01
+  1.43472880e-01  3.92976962e-02  2.07755864e-01 -1.66864038e-01
+ -2.07617655e-01  1.54489219e-01 -2.89462149e-01  1.33851171e-01
+  9.15572327e-03  1.38254583e-01  1.57219321e-01 -1.10909589e-01
+ -3.12280357e-02 -2.14093551e-01 -9.95291397e-02  1.29718438e-01
+  1.03058912e-01  4.53612059e-02 -2.10352883e-01 -4.70763855e-02
+  1.73520684e-01 -1.00697435e-01 -7.36497948e-03  1.75518319e-01
+  5.09812199e-02 -2.00088933e-01 -1.67289600e-01 -1.55999362e-01
+  1.60037607e-01  6.48457259e-02 -2.90617365e-02 -2.07897946e-01
+ -3.88999172e-02 -2.27546189e-02 -1.55136541e-01  1.46816432e-01
+  6.72741607e-02 -1.00608030e-02  6.64832070e-02  2.17609834e-02
+ -9.21988208e-03 -1.51559293e-01  3.19240898e-01  1.57861724e-01
+ -1.44274905e-01  3.62334639e-01  5.82315214e-03  2.03267828e-01
+ -2.63387233e-01 -1.72018845e-04  8.71438440e-03  1.84498206e-01
+  1.15185581e-01  5.37278205e-02  1.30814001e-01  3.53452452e-02
+  1.47847787e-01  1.84367403e-01 -1.18797421e-01 -1.30004659e-01
+ -3.06758851e-01  8.21810123e-03 -2.57283654e-02  2.02897429e-01
+ -1.42591884e-02 -9.96511355e-02  1.40742317e-01  9.23444554e-02
+  6.88763484e-02  4.98412410e-03  1.85781002e-01  1.68066081e-02
+ -4.31126989e-02  4.72450405e-02  2.23643109e-01 -2.07959898e-02
+  1.16742261e-01 -6.73903450e-02  9.41318795e-02  1.67366609e-01]</t>
         </is>
       </c>
       <c r="I3" t="n">
-        <v>0.9850549101829529</v>
+        <v>0.9779635071754456</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
-        <v>65</v>
+        <v>9</v>
       </c>
       <c r="B4" t="n">
-        <v>2023052001854</v>
+        <v>2023046001084</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Flu B PCR</t>
+          <t>SARS-CoV-2 (In-house)</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Influenza virus B RNA Presence Respiratory Specimen NAA Probe Detection</t>
+          <t>SARS Coronavirus 2 N gene Presence Respiratory Specimen NAA Probe Detection</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>['flu', 'b', 'pcr']</t>
+          <t>['sars-cov-2', '(in-house)']</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>['influenza', 'virus', 'b', 'rna', 'presence', 'respiratory', 'specimen', 'naa', 'probe', 'detection']</t>
+          <t>['sars', 'coronavirus', '2', 'n', 'gene', 'presence', 'respiratory', 'specimen', 'naa', 'probe', 'detection']</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>[ 0.0467584   0.0691103   0.09038106  0.135699   -0.0084669  -0.0817739
-  0.12620395  0.20142126 -0.19785589 -0.1861846  -0.05044567 -0.11109995
-  0.06554832  0.05452247  0.0892775  -0.01388188  0.2204675  -0.03774988
- -0.06308102 -0.37479594  0.1141826   0.03134486  0.12696491 -0.14048073
- -0.18278871  0.11085564 -0.20664935  0.10194904  0.0061385   0.10416649
-  0.10020583 -0.0828228  -0.04210684 -0.17210741 -0.07762072  0.09549082
-  0.07580351  0.03151342 -0.17401476 -0.02418203  0.14711435 -0.08841255
-  0.00368272  0.1378382   0.05748519 -0.14606456 -0.13049607 -0.13131012
-  0.13965905  0.04716016 -0.02884331 -0.15109335  0.00309458 -0.01393572
- -0.12548694  0.13751371  0.04892856  0.00329174  0.03560503  0.01767008
-  0.01463552 -0.11503045  0.2014959   0.1280452  -0.08640918  0.2741277
- -0.00627123  0.15831506 -0.17766012  0.00289017  0.00184368  0.11855602
-  0.09029189  0.02638342  0.09677035  0.02617783  0.12287842  0.1460065
- -0.070641   -0.09927804 -0.23731579  0.01257534 -0.0458485   0.1304364
- -0.00167163 -0.06762322  0.0917775   0.08247722  0.06341899  0.00284474
-  0.14685743 -0.00288647 -0.0536647   0.04131594  0.13917947 -0.02124075
-  0.06703387 -0.04754054  0.05822144  0.12540263]</t>
+          <t>[ 0.04099384  0.03036093  0.03719688  0.0723789  -0.00606966 -0.03834537
+  0.06981488  0.10011347 -0.09731035 -0.09967577 -0.02778061 -0.05304503
+  0.04093748  0.03688122  0.05247121 -0.0054679   0.11286175 -0.01439352
+ -0.02683652 -0.17353806  0.05532928  0.01068085  0.04247207 -0.07376201
+ -0.08675149  0.05495713 -0.11086024  0.0451356   0.01849056  0.05317551
+  0.05150653 -0.04630705 -0.02044584 -0.08104759 -0.04514789  0.05058778
+  0.03172289  0.01421874 -0.07712096 -0.02825025  0.06444861 -0.03810681
+  0.01664272  0.08231041  0.01944996 -0.06557912 -0.06922877 -0.07098404
+  0.07728672  0.02141448 -0.02822856 -0.08548534 -0.01351674 -0.01145037
+ -0.04971779  0.08335615  0.02468329  0.00675983  0.03656626  0.00982069
+  0.00618588 -0.05267148  0.10456993  0.06595588 -0.04543399  0.14707218
+ -0.00336928  0.07919807 -0.09339978  0.00158789  0.00232236  0.0543307
+  0.0521557   0.01008676  0.0511211   0.01229559  0.0563812   0.0829775
+ -0.04576359 -0.05852902 -0.12425719  0.00659331 -0.02248363  0.06868609
+  0.01752529 -0.03223506  0.04429378  0.03250644  0.02792649 -0.01478686
+  0.07538357 -0.00343594 -0.02983347  0.04082406  0.05882138 -0.01892258
+  0.0241635  -0.01684863  0.0339029   0.07001537]</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>[ 0.04779003  0.12182136  0.12659077  0.19120806  0.00129924 -0.12661254
-  0.18856426  0.31006068 -0.2852201  -0.26961827 -0.06300162 -0.17960623
-  0.08585751  0.08146276  0.13000615 -0.02610402  0.313487   -0.04039112
- -0.09730656 -0.5422231   0.16544548  0.0452153   0.19197229 -0.18849921
- -0.24858136  0.15738945 -0.2902357   0.1362183   0.00813976  0.13250752
-  0.1518559  -0.13360809 -0.05319064 -0.24639654 -0.10975812  0.14766417
-  0.12900814  0.04752523 -0.24112809 -0.03792614  0.20580712 -0.13291788
- -0.00370827  0.20515399  0.08189792 -0.19420913 -0.19001935 -0.1887528
-  0.19113699  0.06460273 -0.03166019 -0.22146761 -0.00787167 -0.02132439
- -0.17430261  0.17991272  0.09062713 -0.00722372  0.0529852   0.02867844
-  0.00797537 -0.16694924  0.30698806  0.1701334  -0.12463303  0.39291185
- -0.00386158  0.23524413 -0.25902584  0.00808206 -0.00223985  0.17380795
-  0.13860616  0.05172863  0.14603727  0.04026961  0.16966513  0.21445444
- -0.1056105  -0.14369129 -0.34521565  0.01118272 -0.04967145  0.1815639
- -0.00877856 -0.09421234  0.14242953  0.09296162  0.0866642   0.00319975
-  0.20705521  0.01287749 -0.05482947  0.05088411  0.22315142 -0.01830191
-  0.10388656 -0.06538913  0.08039974  0.18420117]</t>
+          <t>[ 0.04662573  0.11959891  0.12047911  0.1755962   0.00536833 -0.1220286
+  0.17801872  0.29739815 -0.2680124  -0.25337183 -0.0629511  -0.17658602
+  0.0718115   0.07999568  0.11573231 -0.0276543   0.29171133 -0.03511989
+ -0.08863812 -0.5142111   0.1617334   0.0406547   0.1806062  -0.17609303
+ -0.24163952  0.15093757 -0.26577246  0.12338214  0.00473587  0.12279093
+  0.14032537 -0.13095796 -0.05782652 -0.24647857 -0.10129288  0.14559282
+  0.12779914  0.04414372 -0.23538475 -0.03330396  0.20548443 -0.13944313
+ -0.00626652  0.20079823  0.08855048 -0.1731686  -0.18711472 -0.18524393
+  0.18433486  0.05794699 -0.02979312 -0.2110479   0.00367782 -0.01757474
+ -0.16950694  0.16952553  0.09042813 -0.01362576  0.0404085   0.02835342
+  0.01385153 -0.16051121  0.281191    0.16122085 -0.10285317  0.37170744
+ -0.00522764  0.23286971 -0.23547372  0.00620041 -0.00328396  0.1625282
+  0.13566476  0.05230827  0.14349435  0.04079083  0.16407573  0.20906396
+ -0.08627092 -0.13664986 -0.3307455   0.00613369 -0.05054608  0.15555616
+ -0.01125875 -0.09037875  0.13658331  0.08549424  0.0831351  -0.00246866
+  0.2023367   0.017227   -0.05076766  0.04479476  0.20753986 -0.01029286
+  0.09212644 -0.0632881   0.06753721  0.1772288 ]</t>
         </is>
       </c>
       <c r="I4" t="n">
-        <v>0.9981325268745422</v>
+        <v>0.9850577712059021</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B5" t="n">
         <v>2023052001854</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>SARSCoV2 PCR</t>
+          <t>Flu B PCR</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -721,7 +729,7 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>['sarscov2', 'pcr']</t>
+          <t>['flu', 'b', 'pcr']</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
@@ -731,151 +739,232 @@
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>[ 0.04844843  0.04097585  0.05468044  0.08553381 -0.00716977 -0.04813135
-  0.06728864  0.10692909 -0.11112896 -0.10656177 -0.0230101  -0.05408479
-  0.03728933  0.02567744  0.05225131 -0.01310833  0.11359774 -0.02536083
- -0.04379391 -0.20970954  0.05115278  0.01152468  0.05966272 -0.08952783
- -0.11237475  0.05254308 -0.11880186  0.06567106  0.00179746  0.06145913
-  0.04120895 -0.04932846 -0.02536362 -0.09699979 -0.04425767  0.04964162
-  0.03558322  0.01398089 -0.10517532 -0.01832247  0.07262772 -0.05072819
-  0.00448497  0.0850666   0.03443414 -0.08297217 -0.06398244 -0.07187065
-  0.07905512  0.03469725 -0.02080063 -0.08831398  0.01699396 -0.00834439
- -0.0770956   0.08191268  0.01804524  0.01130788  0.01631796  0.01247058
-  0.01945864 -0.06136435  0.10083763  0.07152015 -0.04764584  0.15791023
- -0.00419963  0.09927566 -0.10341233 -0.00135141 -0.0010733   0.07133888
-  0.0546882   0.01383678  0.04895714  0.02521466  0.06212893  0.0839916
- -0.03577501 -0.06505462 -0.13253683  0.01738059 -0.0421322   0.06468762
-  0.01047914 -0.03612808  0.04438345  0.04281233  0.0525249   0.00609992
-  0.08187595 -0.00877491 -0.04751872  0.03520389  0.07726085 -0.02106017
-  0.01935691 -0.03133694  0.02572233  0.05919797]</t>
+          <t>[ 0.04675837  0.0691109   0.09038002  0.13569738 -0.00846731 -0.08177403
+  0.1262028   0.2014222  -0.19785555 -0.18618466 -0.05044685 -0.11109962
+  0.06554744  0.05452142  0.08927699 -0.01388329  0.22046746 -0.03774985
+ -0.06308085 -0.37479532  0.11418176  0.03134343  0.12696299 -0.1404801
+ -0.18278964  0.11085412 -0.2066481   0.10195079  0.00613781  0.10416768
+  0.10020459 -0.08282389 -0.04210809 -0.17210953 -0.07762063  0.09549022
+  0.07580464  0.03151402 -0.17401434 -0.02418     0.14711426 -0.08841291
+  0.00368157  0.13784002  0.05748574 -0.14606526 -0.13049556 -0.13130979
+  0.13965999  0.04716078 -0.02884279 -0.15109266  0.00309609 -0.01393613
+ -0.12548779  0.13751435  0.04892937  0.00329197  0.03560429  0.01767114
+  0.01463691 -0.11503053  0.20149511  0.12804484 -0.08640883  0.2741302
+ -0.00626923  0.15831718 -0.17766088  0.00289024  0.0018449   0.11855664
+  0.09029304  0.02638289  0.09677145  0.02618075  0.12288005  0.14600916
+ -0.07064059 -0.09927937 -0.23731875  0.01257642 -0.04584877  0.13043685
+ -0.00167199 -0.06762412  0.0917777   0.08247899  0.06342072  0.00284445
+  0.14685963 -0.0028861  -0.05366473  0.04131574  0.13918132 -0.02124177
+  0.06703391 -0.0475412   0.05822219  0.12540318]</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>[ 0.04779003  0.12182136  0.12659077  0.19120806  0.00129924 -0.12661254
-  0.18856426  0.31006068 -0.2852201  -0.26961827 -0.06300162 -0.17960623
-  0.08585751  0.08146276  0.13000615 -0.02610402  0.313487   -0.04039112
- -0.09730656 -0.5422231   0.16544548  0.0452153   0.19197229 -0.18849921
- -0.24858136  0.15738945 -0.2902357   0.1362183   0.00813976  0.13250752
-  0.1518559  -0.13360809 -0.05319064 -0.24639654 -0.10975812  0.14766417
-  0.12900814  0.04752523 -0.24112809 -0.03792614  0.20580712 -0.13291788
- -0.00370827  0.20515399  0.08189792 -0.19420913 -0.19001935 -0.1887528
-  0.19113699  0.06460273 -0.03166019 -0.22146761 -0.00787167 -0.02132439
- -0.17430261  0.17991272  0.09062713 -0.00722372  0.0529852   0.02867844
-  0.00797537 -0.16694924  0.30698806  0.1701334  -0.12463303  0.39291185
- -0.00386158  0.23524413 -0.25902584  0.00808206 -0.00223985  0.17380795
-  0.13860616  0.05172863  0.14603727  0.04026961  0.16966513  0.21445444
- -0.1056105  -0.14369129 -0.34521565  0.01118272 -0.04967145  0.1815639
- -0.00877856 -0.09421234  0.14242953  0.09296162  0.0866642   0.00319975
-  0.20705521  0.01287749 -0.05482947  0.05088411  0.22315142 -0.01830191
-  0.10388656 -0.06538913  0.08039974  0.18420117]</t>
+          <t>[ 0.04777879  0.12182455  0.12659252  0.19122157  0.00129177 -0.12661478
+  0.18857615  0.31007177 -0.285242   -0.26963496 -0.06300098 -0.17960584
+  0.08586681  0.08145941  0.1300252  -0.02610597  0.31351143 -0.04039845
+ -0.0973176  -0.54225236  0.1654463   0.04522078  0.1919992  -0.18850443
+ -0.24857612  0.15739776 -0.29026386  0.13623023  0.00814013  0.13251999
+  0.151876   -0.1336094  -0.0531824  -0.24639797 -0.10976728  0.14766435
+  0.1290044   0.04753082 -0.24112713 -0.03793853  0.20580141 -0.13290393
+ -0.00370729  0.20514801  0.08188609 -0.19423133 -0.19002041 -0.18874387
+  0.19113705  0.06460917 -0.03166122 -0.22147842 -0.00789151 -0.02132835
+ -0.17430799  0.17991003  0.09062583 -0.00722374  0.05299749  0.0286726
+  0.00796881 -0.1669535   0.30702707  0.17013831 -0.12465836  0.39292705
+ -0.00385345  0.23524794 -0.2590596   0.00807993 -0.00223649  0.17382793
+  0.13860592  0.05172955  0.14603724  0.04026701  0.16966173  0.2144572
+ -0.10563491 -0.14369896 -0.34522146  0.01117757 -0.04966141  0.18159409
+ -0.00877587 -0.09422453  0.14244065  0.09296878  0.08665787  0.00320465
+  0.20705521  0.01287931 -0.05482993  0.05088512  0.22317865 -0.01830481
+  0.10390051 -0.0653942   0.08041795  0.1842075 ]</t>
         </is>
       </c>
       <c r="I5" t="n">
-        <v>0.9877004027366638</v>
+        <v>0.998132050037384</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="B6" t="n">
-        <v>2023050001755</v>
+        <v>2023052001854</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Culture Stool</t>
+          <t>Flu B PCR</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Stool Culture</t>
+          <t>SARS Coronavirus+SARS-like Coronavirus+SARS Coronavirus 2 RNA Presence Resp Spec NAA Probe Detection</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>['culture', 'stool']</t>
+          <t>['flu', 'b', 'pcr']</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>['stool', 'culture']</t>
+          <t>['sars', 'coronavirus+sars-like', 'coronavirus+sars', 'coronavirus', '2', 'rna', 'presence', 'resp', 'spec', 'naa', 'probe', 'detection']</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>[ 0.0408309   0.07235357  0.08079129  0.11908684  0.00157173 -0.07837151
-  0.11224411  0.19824594 -0.1880071  -0.17322552 -0.04868244 -0.1078335
-  0.06054647  0.05537254  0.0834619  -0.01795734  0.21093604 -0.03093044
- -0.06691341 -0.35845286  0.09985381  0.02620846  0.11460354 -0.12551457
- -0.15637006  0.10785254 -0.19903558  0.09250069  0.00888123  0.09335071
-  0.09492745 -0.0792343  -0.04320787 -0.16363478 -0.06626195  0.09596699
-  0.08043022  0.02464475 -0.1532775  -0.02970717  0.12349104 -0.08801222
-  0.00839785  0.13321993  0.04531045 -0.1356697  -0.12722264 -0.11928111
-  0.12103114  0.03809847 -0.02374435 -0.14654693 -0.01543258 -0.01007843
- -0.11248009  0.11230202  0.05093709 -0.0019772   0.03677601  0.01815809
-  0.01039683 -0.11237743  0.20414495  0.12154973 -0.07848206  0.25702715
-  0.00070521  0.14448047 -0.17832115  0.00124049 -0.00244472  0.11639294
-  0.07885221  0.02734829  0.09119686  0.02167823  0.10340269  0.14409783
- -0.06782983 -0.08893871 -0.22234699  0.01249561 -0.03877387  0.12466979
- -0.00809501 -0.05657817  0.0918172   0.07334256  0.05698293  0.00220558
-  0.13152066  0.00999777 -0.03391752  0.04117463  0.14185598 -0.0186728
-  0.06162491 -0.04287851  0.04635394  0.12188055]</t>
+          <t>[ 0.04675837  0.0691109   0.09038002  0.13569738 -0.00846731 -0.08177403
+  0.1262028   0.2014222  -0.19785555 -0.18618466 -0.05044685 -0.11109962
+  0.06554744  0.05452142  0.08927699 -0.01388329  0.22046746 -0.03774985
+ -0.06308085 -0.37479532  0.11418176  0.03134343  0.12696299 -0.1404801
+ -0.18278964  0.11085412 -0.2066481   0.10195079  0.00613781  0.10416768
+  0.10020459 -0.08282389 -0.04210809 -0.17210953 -0.07762063  0.09549022
+  0.07580464  0.03151402 -0.17401434 -0.02418     0.14711426 -0.08841291
+  0.00368157  0.13784002  0.05748574 -0.14606526 -0.13049556 -0.13130979
+  0.13965999  0.04716078 -0.02884279 -0.15109266  0.00309609 -0.01393613
+ -0.12548779  0.13751435  0.04892937  0.00329197  0.03560429  0.01767114
+  0.01463691 -0.11503053  0.20149511  0.12804484 -0.08640883  0.2741302
+ -0.00626923  0.15831718 -0.17766088  0.00289024  0.0018449   0.11855664
+  0.09029304  0.02638289  0.09677145  0.02618075  0.12288005  0.14600916
+ -0.07064059 -0.09927937 -0.23731875  0.01257642 -0.04584877  0.13043685
+ -0.00167199 -0.06762412  0.0917777   0.08247899  0.06342072  0.00284445
+  0.14685963 -0.0028861  -0.05366473  0.04131574  0.13918132 -0.02124177
+  0.06703391 -0.0475412   0.05822219  0.12540318]</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>[ 0.0408309   0.07235357  0.08079129  0.11908684  0.00157173 -0.07837151
-  0.11224411  0.19824594 -0.1880071  -0.17322552 -0.04868244 -0.1078335
-  0.06054647  0.05537254  0.0834619  -0.01795734  0.21093604 -0.03093044
- -0.06691341 -0.35845286  0.09985381  0.02620846  0.11460354 -0.12551457
- -0.15637006  0.10785254 -0.19903558  0.09250069  0.00888123  0.09335071
-  0.09492745 -0.0792343  -0.04320787 -0.16363478 -0.06626195  0.09596699
-  0.08043022  0.02464475 -0.1532775  -0.02970717  0.12349104 -0.08801222
-  0.00839785  0.13321993  0.04531045 -0.1356697  -0.12722264 -0.11928111
-  0.12103114  0.03809847 -0.02374435 -0.14654693 -0.01543258 -0.01007843
- -0.11248009  0.11230202  0.05093709 -0.0019772   0.03677601  0.01815809
-  0.01039683 -0.11237743  0.20414495  0.12154973 -0.07848206  0.25702715
-  0.00070521  0.14448047 -0.17832115  0.00124049 -0.00244472  0.11639294
-  0.07885221  0.02734829  0.09119686  0.02167823  0.10340269  0.14409783
- -0.06782983 -0.08893871 -0.22234699  0.01249561 -0.03877387  0.12466979
- -0.00809501 -0.05657817  0.0918172   0.07334256  0.05698293  0.00220558
-  0.13152066  0.00999777 -0.03391752  0.04117463  0.14185598 -0.0186728
-  0.06162491 -0.04287851  0.04635394  0.12188055]</t>
+          <t>[ 2.99221147e-02  1.03954159e-01  1.15190476e-01  1.70237735e-01
+ -9.24916286e-03 -1.16083525e-01  1.71648994e-01  2.88631946e-01
+ -2.73772031e-01 -2.61409819e-01 -5.14109731e-02 -1.57738686e-01
+  8.54621902e-02  6.48749918e-02  1.36029750e-01 -2.11676061e-02
+  3.07783931e-01 -4.42240126e-02 -8.93947780e-02 -5.12431681e-01
+  1.43472880e-01  3.92976962e-02  2.07755864e-01 -1.66864038e-01
+ -2.07617655e-01  1.54489219e-01 -2.89462149e-01  1.33851171e-01
+  9.15572327e-03  1.38254583e-01  1.57219321e-01 -1.10909589e-01
+ -3.12280357e-02 -2.14093551e-01 -9.95291397e-02  1.29718438e-01
+  1.03058912e-01  4.53612059e-02 -2.10352883e-01 -4.70763855e-02
+  1.73520684e-01 -1.00697435e-01 -7.36497948e-03  1.75518319e-01
+  5.09812199e-02 -2.00088933e-01 -1.67289600e-01 -1.55999362e-01
+  1.60037607e-01  6.48457259e-02 -2.90617365e-02 -2.07897946e-01
+ -3.88999172e-02 -2.27546189e-02 -1.55136541e-01  1.46816432e-01
+  6.72741607e-02 -1.00608030e-02  6.64832070e-02  2.17609834e-02
+ -9.21988208e-03 -1.51559293e-01  3.19240898e-01  1.57861724e-01
+ -1.44274905e-01  3.62334639e-01  5.82315214e-03  2.03267828e-01
+ -2.63387233e-01 -1.72018845e-04  8.71438440e-03  1.84498206e-01
+  1.15185581e-01  5.37278205e-02  1.30814001e-01  3.53452452e-02
+  1.47847787e-01  1.84367403e-01 -1.18797421e-01 -1.30004659e-01
+ -3.06758851e-01  8.21810123e-03 -2.57283654e-02  2.02897429e-01
+ -1.42591884e-02 -9.96511355e-02  1.40742317e-01  9.23444554e-02
+  6.88763484e-02  4.98412410e-03  1.85781002e-01  1.68066081e-02
+ -4.31126989e-02  4.72450405e-02  2.23643109e-01 -2.07959898e-02
+  1.16742261e-01 -6.73903450e-02  9.41318795e-02  1.67366609e-01]</t>
         </is>
       </c>
       <c r="I6" t="n">
-        <v>0.9999999403953552</v>
+        <v>0.9935986399650574</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
+        <v>75</v>
+      </c>
+      <c r="B7" t="n">
+        <v>2023050001755</v>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Culture Stool</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Stool Culture</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>['culture', 'stool']</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>['stool', 'culture']</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>[ 0.04082959  0.07235076  0.08078685  0.11908036  0.00157193 -0.07836786
+  0.11223817  0.1982376  -0.18799892 -0.17321756 -0.04868115 -0.10782814
+  0.06054386  0.05536949  0.08345804 -0.0179575   0.21092725 -0.03092903
+ -0.06691091 -0.3584371   0.09984881  0.02620621  0.11459702 -0.12550908
+ -0.15636355  0.10784693 -0.19902585  0.09249766  0.00888027  0.09334747
+  0.09492238 -0.07923122 -0.04320741 -0.16362932 -0.06625875  0.09596248
+  0.0804273   0.02464394 -0.15327057 -0.02970481  0.12348518 -0.08800887
+  0.00839741  0.13321522  0.04530902 -0.13566428 -0.12721696 -0.11927561
+  0.1210262   0.0380969  -0.02374305 -0.14653969 -0.01543147 -0.01007852
+ -0.11247588  0.11229686  0.0509349  -0.00197702  0.0367734   0.0181577
+  0.01039767 -0.1123728   0.20413554  0.1215447  -0.07847869  0.2570184
+  0.0007065   0.1444758  -0.17831488  0.00124025 -0.0024438   0.11638875
+  0.07884924  0.02734697  0.09119358  0.02167891  0.10339972  0.1440939
+ -0.06782672 -0.08893549 -0.22233948  0.01249581 -0.03877292  0.12466505
+ -0.00809504 -0.05657632  0.09181384  0.07334124  0.05698184  0.00220524
+  0.13151643  0.00999778 -0.03391563  0.04117304  0.14185157 -0.01867266
+  0.06162238 -0.04287735  0.04635227  0.12187567]</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>[ 0.04082959  0.07235076  0.08078685  0.11908036  0.00157193 -0.07836786
+  0.11223817  0.1982376  -0.18799892 -0.17321756 -0.04868115 -0.10782814
+  0.06054386  0.05536949  0.08345804 -0.0179575   0.21092725 -0.03092903
+ -0.06691091 -0.3584371   0.09984881  0.02620621  0.11459702 -0.12550908
+ -0.15636355  0.10784693 -0.19902585  0.09249766  0.00888027  0.09334747
+  0.09492238 -0.07923122 -0.04320741 -0.16362932 -0.06625875  0.09596248
+  0.0804273   0.02464394 -0.15327057 -0.02970481  0.12348518 -0.08800887
+  0.00839741  0.13321522  0.04530902 -0.13566428 -0.12721696 -0.11927561
+  0.1210262   0.0380969  -0.02374305 -0.14653969 -0.01543147 -0.01007852
+ -0.11247588  0.11229686  0.0509349  -0.00197702  0.0367734   0.0181577
+  0.01039767 -0.1123728   0.20413554  0.1215447  -0.07847869  0.2570184
+  0.0007065   0.1444758  -0.17831488  0.00124025 -0.0024438   0.11638875
+  0.07884924  0.02734697  0.09119358  0.02167891  0.10339972  0.1440939
+ -0.06782672 -0.08893549 -0.22233948  0.01249581 -0.03877292  0.12466505
+ -0.00809504 -0.05657632  0.09181384  0.07334124  0.05698184  0.00220524
+  0.13151643  0.00999778 -0.03391563  0.04117304  0.14185157 -0.01867266
+  0.06162238 -0.04287735  0.04635227  0.12187567]</t>
+        </is>
+      </c>
+      <c r="I7" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="n">
         <v>80</v>
       </c>
-      <c r="B7" t="n">
+      <c r="B8" t="n">
         <v>2023050000939</v>
       </c>
-      <c r="C7" t="inlineStr">
+      <c r="C8" t="inlineStr">
         <is>
           <t>nan</t>
         </is>
       </c>
-      <c r="D7" t="inlineStr">
+      <c r="D8" t="inlineStr">
         <is>
           <t>nan</t>
         </is>
       </c>
-      <c r="E7" t="inlineStr">
+      <c r="E8" t="inlineStr">
         <is>
           <t>['nan']</t>
         </is>
       </c>
-      <c r="F7" t="inlineStr">
+      <c r="F8" t="inlineStr">
         <is>
           <t>['nan']</t>
         </is>
       </c>
-      <c r="G7" t="inlineStr">
+      <c r="G8" t="inlineStr">
         <is>
           <t>[ 1.3325238e-03  6.5408563e-03  9.9846032e-03  9.0624550e-03
  -8.0153607e-03  6.4913859e-03 -5.7147373e-03 -9.7157480e-04
@@ -904,7 +993,7 @@
  -5.2507855e-03  9.0599954e-03 -5.7907687e-03  3.6860751e-03]</t>
         </is>
       </c>
-      <c r="H7" t="inlineStr">
+      <c r="H8" t="inlineStr">
         <is>
           <t>[ 1.3325238e-03  6.5408563e-03  9.9846032e-03  9.0624550e-03
  -8.0153607e-03  6.4913859e-03 -5.7147373e-03 -9.7157480e-04
@@ -933,170 +1022,259 @@
  -5.2507855e-03  9.0599954e-03 -5.7907687e-03  3.6860751e-03]</t>
         </is>
       </c>
-      <c r="I7" t="n">
+      <c r="I8" t="n">
         <v>0.9999999403953552</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="1" t="n">
-        <v>193</v>
-      </c>
-      <c r="B8" t="n">
-        <v>2023051002782</v>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>Flu A PCR</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>Influenza virus A RNA Presence Respiratory Specimen NAA Probe Detection</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>['flu', 'a', 'pcr']</t>
-        </is>
-      </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>['influenza', 'virus', 'a', 'rna', 'presence', 'respiratory', 'specimen', 'naa', 'probe', 'detection']</t>
-        </is>
-      </c>
-      <c r="G8" t="inlineStr">
-        <is>
-          <t>[ 4.96691130e-02  7.38299936e-02  9.63081121e-02  1.40820265e-01
- -1.01992972e-02 -8.79303217e-02  1.26648396e-01  2.08529010e-01
- -2.02009514e-01 -1.97193980e-01 -5.23451716e-02 -1.19633347e-01
-  6.74114376e-02  5.78540303e-02  9.72970724e-02 -1.15495017e-02
-  2.22599819e-01 -3.55063044e-02 -6.27056435e-02 -3.83009672e-01
-  1.15860872e-01  3.54168713e-02  1.24908924e-01 -1.39447212e-01
- -1.82346240e-01  1.19997650e-01 -2.14240670e-01  1.05489962e-01
-  8.43307469e-03  1.03498995e-01  1.00253515e-01 -8.49479958e-02
- -4.65214439e-02 -1.81823030e-01 -7.78433383e-02  9.87588540e-02
-  8.44045281e-02  3.01631037e-02 -1.82102382e-01 -2.17489246e-02
-  1.51285544e-01 -9.16479453e-02  1.34920049e-03  1.40516147e-01
-  5.81736229e-02 -1.50163904e-01 -1.36153102e-01 -1.33075103e-01
-  1.40180543e-01  4.64790314e-02 -2.71225516e-02 -1.58266068e-01
-  9.07215581e-04 -1.21578574e-02 -1.27360865e-01  1.42708704e-01
-  4.90422063e-02  1.85897446e-03  3.97594161e-02  2.11824477e-02
-  1.17762154e-02 -1.17030822e-01  2.09159195e-01  1.35410160e-01
- -8.36701989e-02  2.82843441e-01 -9.72119812e-03  1.63591981e-01
- -1.81932077e-01  4.21468774e-03 -3.44086293e-04  1.24772847e-01
-  9.29786563e-02  2.54743695e-02  9.82622728e-02  3.22718322e-02
-  1.21003740e-01  1.48842737e-01 -7.07208961e-02 -1.02248885e-01
- -2.47144878e-01  1.13230385e-02 -4.32354324e-02  1.29271522e-01
- -3.01450421e-03 -6.58600330e-02  9.78473052e-02  8.19147825e-02
-  6.78882748e-02  2.91710906e-03  1.49054199e-01 -1.06038246e-03
- -5.70910685e-02  4.60759513e-02  1.46546349e-01 -2.17806567e-02
-  6.75330460e-02 -4.96821664e-02  5.79851754e-02  1.31460190e-01]</t>
-        </is>
-      </c>
-      <c r="H8" t="inlineStr">
-        <is>
-          <t>[ 0.04866324  0.12323727  0.12836888  0.19274443  0.00077953 -0.12845947
-  0.18869759  0.312193   -0.28646618 -0.2729211  -0.06357147 -0.18216625
-  0.08641645  0.08246223  0.13241202 -0.02540431  0.31412673 -0.03971805
- -0.09719395 -0.5446873   0.16594897  0.04643691  0.1913555  -0.18818916
- -0.24844864  0.16013205 -0.29251307  0.13728057  0.00882813  0.13230726
-  0.15187022 -0.13424566 -0.05451502 -0.24931121 -0.10982491  0.14864458
-  0.13158843  0.04712014 -0.24355438 -0.03719621  0.20705846 -0.1338885
- -0.00440832  0.20595737  0.08210445 -0.1954389  -0.19171646 -0.1892823
-  0.19129345  0.06439839 -0.03114396 -0.22361943 -0.00852787 -0.02079103
- -0.1748648   0.1814712   0.09066122 -0.00765355  0.05423152  0.02973215
-  0.00711758 -0.16754936  0.30928707  0.1723429  -0.12381134  0.3955266
- -0.00489657  0.23682721 -0.2603074   0.00847942 -0.00289618  0.17567301
-  0.13941216  0.05145591  0.14648485  0.04209781  0.16910271  0.2153053
- -0.10563447 -0.14458254 -0.3481644   0.01080703 -0.04888753  0.18121442
- -0.00918142 -0.09368338  0.14425047  0.09279289  0.08800498  0.00322146
-  0.20771424  0.01342532 -0.05585738  0.05231212  0.2253615  -0.01846388
-  0.10403632 -0.06603162  0.08032886  0.18601842]</t>
-        </is>
-      </c>
-      <c r="I8" t="n">
-        <v>0.9982849955558777</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
+        <v>193</v>
+      </c>
+      <c r="B9" t="n">
+        <v>2023051002782</v>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Flu A PCR</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>Influenza virus A RNA Presence Respiratory Specimen NAA Probe Detection</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>['flu', 'a', 'pcr']</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>['influenza', 'virus', 'a', 'rna', 'presence', 'respiratory', 'specimen', 'naa', 'probe', 'detection']</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>[ 4.96681780e-02  7.38294274e-02  9.63056162e-02  1.40816644e-01
+ -1.01996763e-02 -8.79289508e-02  1.26645371e-01  2.08526656e-01
+ -2.02006042e-01 -1.97191104e-01 -5.23454733e-02 -1.19631074e-01
+  6.74095899e-02  5.78517579e-02  9.72952917e-02 -1.15507962e-02
+  2.22596273e-01 -3.55060101e-02 -6.27050698e-02 -3.83002996e-01
+  1.15858175e-01  3.54152322e-02  1.24905102e-01 -1.39444426e-01
+ -1.82344079e-01  1.19994126e-01 -2.14235887e-01  1.05490185e-01
+  8.43212008e-03  1.03498697e-01  1.00250594e-01 -8.49479958e-02
+ -4.65222038e-02 -1.81822672e-01 -7.78423399e-02  9.87564623e-02
+  8.44046175e-02  3.01633254e-02 -1.82099000e-01 -2.17466038e-02
+  1.51282758e-01 -9.16463807e-02  1.34807825e-03  1.40515253e-01
+  5.81732690e-02 -1.50162414e-01 -1.36150315e-01 -1.33072004e-01
+  1.40179321e-01  4.64792848e-02 -2.71216240e-02 -1.58262908e-01
+  9.08562273e-04 -1.21582644e-02 -1.27359957e-01  1.42707184e-01
+  4.90424223e-02  1.85933767e-03  3.97577845e-02  2.11830661e-02
+  1.17776133e-02 -1.17028855e-01  2.09155366e-01  1.35407642e-01
+ -8.36695656e-02  2.82843858e-01 -9.71886236e-03  1.63592830e-01
+ -1.81932077e-01  4.21461230e-03 -3.42432264e-04  1.24772824e-01
+  9.29792002e-02  2.54733413e-02  9.82621312e-02  3.22742164e-02
+  1.21004343e-01  1.48843959e-01 -7.07205832e-02 -1.02249376e-01
+ -2.47145593e-01  1.13239093e-02 -4.32351828e-02  1.29271224e-01
+ -3.01471422e-03 -6.58606067e-02  9.78468060e-02  8.19160566e-02
+  6.78891912e-02  2.91695632e-03  1.49054989e-01 -1.05991296e-03
+ -5.70904613e-02  4.60753143e-02  1.46547899e-01 -2.17812508e-02
+  6.75324425e-02 -4.96826619e-02  5.79857416e-02  1.31459594e-01]</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>[ 0.04865173  0.12324011  0.1283702   0.19275734  0.00077206 -0.12846127
+  0.18870893  0.3122031  -0.28648713 -0.27293688 -0.06357057 -0.1821653
+  0.08642545  0.08245851  0.13243069 -0.02540622  0.31415007 -0.0397253
+ -0.09720486 -0.54471475  0.16594921  0.04644232  0.19138183 -0.18819374
+ -0.24844246  0.16013977 -0.2925402   0.13729206  0.00882842  0.1323193
+  0.1518898  -0.13424663 -0.05450664 -0.24931192 -0.1098338   0.14864424
+  0.1315844   0.04712561 -0.24355254 -0.03720851  0.20705196 -0.13387397
+ -0.00440734  0.20595057  0.08209235 -0.19546047 -0.19171682 -0.18927254
+  0.19129285  0.06440472 -0.03114487 -0.22362947 -0.00854777 -0.02079499
+ -0.17486966  0.18146789  0.09065975 -0.00765353  0.05424354  0.02972618
+  0.00711102 -0.167553    0.30932516  0.17234716 -0.12383658  0.39554116
+ -0.00488834  0.23683064 -0.260341    0.00847724 -0.00289269  0.17569278
+  0.13941178  0.05145669  0.14648443  0.04209504  0.169099    0.21530767
+ -0.1056589  -0.14458995 -0.3481695   0.01080182 -0.04887734  0.1812444
+ -0.00917869 -0.09369548  0.14426139  0.0927999   0.08799841  0.00322641
+  0.20771381  0.01342717 -0.05585765  0.05231299  0.22538862 -0.01846665
+  0.10405006 -0.06603664  0.08034702  0.18602443]</t>
+        </is>
+      </c>
+      <c r="I9" t="n">
+        <v>0.9982843995094299</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="n">
+        <v>194</v>
+      </c>
+      <c r="B10" t="n">
+        <v>2023051002782</v>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Flu A PCR</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>SARS Coronavirus+SARS-like Coronavirus+SARS Coronavirus 2 RNA Presence Resp Spec NAA Probe Detection</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>['flu', 'a', 'pcr']</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>['sars', 'coronavirus+sars-like', 'coronavirus+sars', 'coronavirus', '2', 'rna', 'presence', 'resp', 'spec', 'naa', 'probe', 'detection']</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>[ 4.96681780e-02  7.38294274e-02  9.63056162e-02  1.40816644e-01
+ -1.01996763e-02 -8.79289508e-02  1.26645371e-01  2.08526656e-01
+ -2.02006042e-01 -1.97191104e-01 -5.23454733e-02 -1.19631074e-01
+  6.74095899e-02  5.78517579e-02  9.72952917e-02 -1.15507962e-02
+  2.22596273e-01 -3.55060101e-02 -6.27050698e-02 -3.83002996e-01
+  1.15858175e-01  3.54152322e-02  1.24905102e-01 -1.39444426e-01
+ -1.82344079e-01  1.19994126e-01 -2.14235887e-01  1.05490185e-01
+  8.43212008e-03  1.03498697e-01  1.00250594e-01 -8.49479958e-02
+ -4.65222038e-02 -1.81822672e-01 -7.78423399e-02  9.87564623e-02
+  8.44046175e-02  3.01633254e-02 -1.82099000e-01 -2.17466038e-02
+  1.51282758e-01 -9.16463807e-02  1.34807825e-03  1.40515253e-01
+  5.81732690e-02 -1.50162414e-01 -1.36150315e-01 -1.33072004e-01
+  1.40179321e-01  4.64792848e-02 -2.71216240e-02 -1.58262908e-01
+  9.08562273e-04 -1.21582644e-02 -1.27359957e-01  1.42707184e-01
+  4.90424223e-02  1.85933767e-03  3.97577845e-02  2.11830661e-02
+  1.17776133e-02 -1.17028855e-01  2.09155366e-01  1.35407642e-01
+ -8.36695656e-02  2.82843858e-01 -9.71886236e-03  1.63592830e-01
+ -1.81932077e-01  4.21461230e-03 -3.42432264e-04  1.24772824e-01
+  9.29792002e-02  2.54733413e-02  9.82621312e-02  3.22742164e-02
+  1.21004343e-01  1.48843959e-01 -7.07205832e-02 -1.02249376e-01
+ -2.47145593e-01  1.13239093e-02 -4.32351828e-02  1.29271224e-01
+ -3.01471422e-03 -6.58606067e-02  9.78468060e-02  8.19160566e-02
+  6.78891912e-02  2.91695632e-03  1.49054989e-01 -1.05991296e-03
+ -5.70904613e-02  4.60753143e-02  1.46547899e-01 -2.17812508e-02
+  6.75324425e-02 -4.96826619e-02  5.79857416e-02  1.31459594e-01]</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>[ 2.99221147e-02  1.03954159e-01  1.15190476e-01  1.70237735e-01
+ -9.24916286e-03 -1.16083525e-01  1.71648994e-01  2.88631946e-01
+ -2.73772031e-01 -2.61409819e-01 -5.14109731e-02 -1.57738686e-01
+  8.54621902e-02  6.48749918e-02  1.36029750e-01 -2.11676061e-02
+  3.07783931e-01 -4.42240126e-02 -8.93947780e-02 -5.12431681e-01
+  1.43472880e-01  3.92976962e-02  2.07755864e-01 -1.66864038e-01
+ -2.07617655e-01  1.54489219e-01 -2.89462149e-01  1.33851171e-01
+  9.15572327e-03  1.38254583e-01  1.57219321e-01 -1.10909589e-01
+ -3.12280357e-02 -2.14093551e-01 -9.95291397e-02  1.29718438e-01
+  1.03058912e-01  4.53612059e-02 -2.10352883e-01 -4.70763855e-02
+  1.73520684e-01 -1.00697435e-01 -7.36497948e-03  1.75518319e-01
+  5.09812199e-02 -2.00088933e-01 -1.67289600e-01 -1.55999362e-01
+  1.60037607e-01  6.48457259e-02 -2.90617365e-02 -2.07897946e-01
+ -3.88999172e-02 -2.27546189e-02 -1.55136541e-01  1.46816432e-01
+  6.72741607e-02 -1.00608030e-02  6.64832070e-02  2.17609834e-02
+ -9.21988208e-03 -1.51559293e-01  3.19240898e-01  1.57861724e-01
+ -1.44274905e-01  3.62334639e-01  5.82315214e-03  2.03267828e-01
+ -2.63387233e-01 -1.72018845e-04  8.71438440e-03  1.84498206e-01
+  1.15185581e-01  5.37278205e-02  1.30814001e-01  3.53452452e-02
+  1.47847787e-01  1.84367403e-01 -1.18797421e-01 -1.30004659e-01
+ -3.06758851e-01  8.21810123e-03 -2.57283654e-02  2.02897429e-01
+ -1.42591884e-02 -9.96511355e-02  1.40742317e-01  9.23444554e-02
+  6.88763484e-02  4.98412410e-03  1.85781002e-01  1.68066081e-02
+ -4.31126989e-02  4.72450405e-02  2.23643109e-01 -2.07959898e-02
+  1.16742261e-01 -6.73903450e-02  9.41318795e-02  1.67366609e-01]</t>
+        </is>
+      </c>
+      <c r="I10" t="n">
+        <v>0.99348384141922</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="n">
         <v>915</v>
       </c>
-      <c r="B9" t="n">
+      <c r="B11" t="n">
         <v>2023030002040</v>
       </c>
-      <c r="C9" t="inlineStr">
+      <c r="C11" t="inlineStr">
         <is>
           <t>Culture AFB with AFB Stain</t>
         </is>
       </c>
-      <c r="D9" t="inlineStr">
+      <c r="D11" t="inlineStr">
         <is>
           <t>AFB Culture</t>
         </is>
       </c>
-      <c r="E9" t="inlineStr">
+      <c r="E11" t="inlineStr">
         <is>
           <t>['culture', 'afb', 'with', 'afb', 'stain']</t>
         </is>
       </c>
-      <c r="F9" t="inlineStr">
+      <c r="F11" t="inlineStr">
         <is>
           <t>['afb', 'culture']</t>
         </is>
       </c>
-      <c r="G9" t="inlineStr">
-        <is>
-          <t>[ 0.04427572  0.08253935  0.08908961  0.13660158 -0.00631126 -0.08636904
-  0.13034017  0.21640824 -0.19565715 -0.18650585 -0.0495294  -0.12223306
-  0.06462695  0.04963094  0.08837844 -0.02289165  0.2229225  -0.03542683
- -0.06207973 -0.38475063  0.11670937  0.0220036   0.12540406 -0.1338026
- -0.17498606  0.11365893 -0.21573357  0.09624132  0.00474488  0.09413281
-  0.11016626 -0.08817229 -0.03565587 -0.17899786 -0.07305562  0.09611785
-  0.08982054  0.03484901 -0.17232187 -0.02832465  0.13450848 -0.09744543
-  0.00440982  0.14401965  0.04371187 -0.15150625 -0.12510587 -0.13073765
-  0.13229632  0.04675937 -0.02859732 -0.15697561 -0.01071095 -0.00693909
- -0.12428892  0.12673831  0.05659807 -0.00895575  0.03127657  0.02500586
-  0.01367202 -0.11900041  0.22174074  0.12577835 -0.09039342  0.27652946
- -0.00203878  0.16194808 -0.18616734 -0.00578116 -0.00169672  0.12124619
-  0.09435707  0.03186367  0.10654929  0.02900942  0.10921907  0.15689653
- -0.07280181 -0.10151687 -0.24029343  0.01086688 -0.04068282  0.13561606
- -0.01253498 -0.07039851  0.10233708  0.07390303  0.06403479 -0.00072173
-  0.14314039  0.00807568 -0.03606218  0.04170726  0.1589794  -0.01866061
-  0.06157005 -0.04535367  0.04911157  0.12620041]</t>
-        </is>
-      </c>
-      <c r="H9" t="inlineStr">
-        <is>
-          <t>[ 4.71463613e-02  8.58654231e-02  9.13902074e-02  1.38233334e-01
- -5.73348161e-03 -8.86498541e-02  1.31453127e-01  2.22669989e-01
- -2.01025009e-01 -1.91491544e-01 -5.18367402e-02 -1.22430012e-01
-  6.57207370e-02  5.25465421e-02  8.95233154e-02 -2.09752023e-02
-  2.29782730e-01 -3.34076211e-02 -6.61728978e-02 -3.95103306e-01
-  1.17023170e-01  2.41717938e-02  1.27966449e-01 -1.39054924e-01
- -1.79620460e-01  1.16432965e-01 -2.22136647e-01  9.79688317e-02
-  6.06717076e-03  9.95624661e-02  1.12190515e-01 -9.09186825e-02
- -3.90620083e-02 -1.83504522e-01 -7.58531690e-02  1.02024786e-01
-  9.17287022e-02  3.44892815e-02 -1.75648272e-01 -3.23767699e-02
-  1.39076740e-01 -9.93470699e-02  5.17144054e-03  1.47010177e-01
-  4.57721241e-02 -1.55216575e-01 -1.30298212e-01 -1.36051252e-01
-  1.35455757e-01  4.67822477e-02 -2.91563645e-02 -1.62050247e-01
- -1.25465728e-02 -9.25974641e-03 -1.26210496e-01  1.29147097e-01
-  5.56526445e-02 -8.66314955e-03  3.20161656e-02  2.38727480e-02
-  1.38973128e-02 -1.21799111e-01  2.26787627e-01  1.29626274e-01
- -9.01330858e-02  2.85021991e-01  4.42293473e-04  1.63586348e-01
- -1.92528114e-01 -5.56362327e-03 -3.11824353e-03  1.23289205e-01
-  9.44482312e-02  3.25851031e-02  1.08270980e-01  2.90855337e-02
-  1.11251920e-01  1.60449311e-01 -7.49821216e-02 -1.02733038e-01
- -2.44275510e-01  1.29968533e-02 -4.09156494e-02  1.38811693e-01
- -1.18994666e-02 -7.08496496e-02  1.05181262e-01  7.72853047e-02
-  6.40407354e-02  2.85187387e-04  1.45982742e-01  7.42449332e-03
- -3.67263593e-02  4.17479798e-02  1.60900995e-01 -2.15013772e-02
-  6.27152622e-02 -4.46208417e-02  5.09194732e-02  1.31402716e-01]</t>
-        </is>
-      </c>
-      <c r="I9" t="n">
-        <v>0.9999237060546875</v>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>[ 0.04427262  0.08253208  0.08908113  0.13658832 -0.00631105 -0.08636088
+  0.13032764  0.21638887 -0.1956383  -0.18648815 -0.04952559 -0.12222159
+  0.06462111  0.04962519  0.08836953 -0.02289081  0.22290206 -0.03542382
+ -0.06207372 -0.384715    0.1166985   0.02200007  0.12539057 -0.13379025
+ -0.1749707   0.11364775 -0.21571322  0.09623318  0.00474376  0.09412435
+  0.11015537 -0.08816452 -0.03565328 -0.17898315 -0.0730485   0.09610805
+  0.08981329  0.03484612 -0.1723063  -0.0283208   0.13449524 -0.09743728
+  0.00440942  0.14400727  0.04370746 -0.15149347 -0.1250933  -0.13072544
+  0.1322844   0.04675538 -0.02859488 -0.15696044 -0.01070935 -0.00693832
+ -0.12427814  0.12672684  0.05659295 -0.00895515  0.03127228  0.02500466
+  0.0136722  -0.1189898   0.22171985  0.12576687 -0.09038529  0.27650586
+ -0.00203775  0.16193458 -0.18615119 -0.00578149 -0.00169591  0.12123527
+  0.09434921  0.03186037  0.10654058  0.02900825  0.10920984  0.15688424
+ -0.07279494 -0.10150824 -0.24027324  0.01086685 -0.04068002  0.13560449
+ -0.01253484 -0.07039277  0.10232839  0.07389782  0.06403032 -0.00072197
+  0.14312844  0.00807499 -0.03605834  0.04170361  0.15896642 -0.01865949
+  0.06156375 -0.04534991  0.04910674  0.1261888 ]</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>[ 4.71430197e-02  8.58581960e-02  9.13815126e-02  1.38219878e-01
+ -5.73320314e-03 -8.86416212e-02  1.31440520e-01  2.22650483e-01
+ -2.01006055e-01 -1.91473708e-01 -5.18328734e-02 -1.22418389e-01
+  6.57148063e-02  5.25406227e-02  8.95144269e-02 -2.09744032e-02
+  2.29762226e-01 -3.34046073e-02 -6.61669075e-02 -3.95067424e-01
+  1.17012218e-01  2.41682008e-02  1.27953038e-01 -1.39042377e-01
+ -1.79604843e-01  1.16421655e-01 -2.22116083e-01  9.79606658e-02
+  6.06594887e-03  9.95539725e-02  1.12179659e-01 -9.09108371e-02
+ -3.90594192e-02 -1.83489799e-01 -7.58459866e-02  1.02014862e-01
+  9.17213857e-02  3.44864726e-02 -1.75632447e-01 -3.23728807e-02
+  1.39063358e-01 -9.93387625e-02  5.17101586e-03  1.46997601e-01
+  4.57677096e-02 -1.55203730e-01 -1.30285487e-01 -1.36038810e-01
+  1.35443687e-01  4.67782766e-02 -2.91538015e-02 -1.62034869e-01
+ -1.25450836e-02 -9.25907120e-03 -1.26199663e-01  1.29135311e-01
+  5.56474924e-02 -8.66260938e-03  3.20117585e-02  2.38714535e-02
+  1.38975047e-02 -1.21788383e-01  2.26766765e-01  1.29614681e-01
+ -9.01248530e-02  2.84998000e-01  4.43483703e-04  1.63572699e-01
+ -1.92511827e-01 -5.56400698e-03 -3.11735831e-03  1.23278178e-01
+  9.44401994e-02  3.25817987e-02  1.08262107e-01  2.90843397e-02
+  1.11242533e-01  1.60436913e-01 -7.49751478e-02 -1.02724284e-01
+ -2.44254947e-01  1.29967164e-02 -4.09126878e-02  1.38799936e-01
+ -1.18993213e-02 -7.08439499e-02  1.05172552e-01  7.72800744e-02
+  6.40361235e-02  2.84890062e-04  1.45970538e-01  7.42389448e-03
+ -3.67222950e-02  4.17441987e-02  1.60888076e-01 -2.15002112e-02
+  6.27088994e-02 -4.46170866e-02  5.09146154e-02  1.31390899e-01]</t>
+        </is>
+      </c>
+      <c r="I11" t="n">
+        <v>0.9999235868453979</v>
       </c>
     </row>
   </sheetData>

</xml_diff>